<commit_message>
Added capability for ELN file
</commit_message>
<xml_diff>
--- a/modules/SSF00607.xlsx
+++ b/modules/SSF00607.xlsx
@@ -438,52 +438,52 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Unique_Id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Induction Sample Id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Sample Type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Harvest Sample Id</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Strain</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Induction Temp</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Proprionate (Mm)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Arabinose (Um)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Od600</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Plate_Well_Id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Induction Sample Id</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Sample Type</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Harvest Sample Id</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Strain</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Induction Temp</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Proprionate (Mm)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Arabinose (Um)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Od600</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 13</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -590,7 +590,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>P1-A01</t>
+          <t>SSF00607-P1-A01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -625,7 +625,11 @@
       <c r="I2" t="n">
         <v>2.51</v>
       </c>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>P1-A01</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
           <t>P1</t>
@@ -694,7 +698,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>P1-A02</t>
+          <t>SSF00607-P1-A02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -729,7 +733,11 @@
       <c r="I3" t="n">
         <v>2.64</v>
       </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>P1-A02</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>P1</t>
@@ -798,7 +806,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>P1-A03</t>
+          <t>SSF00607-P1-A03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -833,7 +841,11 @@
       <c r="I4" t="n">
         <v>3.1</v>
       </c>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>P1-A03</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>P1</t>
@@ -902,7 +914,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>P1-A04</t>
+          <t>SSF00607-P1-A04</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -937,7 +949,11 @@
       <c r="I5" t="n">
         <v>3.04</v>
       </c>
-      <c r="J5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>P1-A04</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>P1</t>
@@ -1006,7 +1022,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>P1-A05</t>
+          <t>SSF00607-P1-A05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1041,7 +1057,11 @@
       <c r="I6" t="n">
         <v>2.58</v>
       </c>
-      <c r="J6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>P1-A05</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>P1</t>
@@ -1110,7 +1130,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>P1-A06</t>
+          <t>SSF00607-P1-A06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1145,7 +1165,11 @@
       <c r="I7" t="n">
         <v>4.86</v>
       </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>P1-A06</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>P1</t>
@@ -1214,7 +1238,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>P1-A07</t>
+          <t>SSF00607-P1-A07</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1249,7 +1273,11 @@
       <c r="I8" t="n">
         <v>3.21</v>
       </c>
-      <c r="J8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>P1-A07</t>
+        </is>
+      </c>
       <c r="K8" t="inlineStr">
         <is>
           <t>P1</t>
@@ -1318,7 +1346,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>P1-A08</t>
+          <t>SSF00607-P1-A08</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1353,7 +1381,11 @@
       <c r="I9" t="n">
         <v>4.03</v>
       </c>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>P1-A08</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr">
         <is>
           <t>P1</t>
@@ -1422,7 +1454,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>P1-A09</t>
+          <t>SSF00607-P1-A09</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1457,7 +1489,11 @@
       <c r="I10" t="n">
         <v>4.77</v>
       </c>
-      <c r="J10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>P1-A09</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
           <t>P1</t>
@@ -1526,7 +1562,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>P1-A10</t>
+          <t>SSF00607-P1-A10</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1561,7 +1597,11 @@
       <c r="I11" t="n">
         <v>3.9</v>
       </c>
-      <c r="J11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>P1-A10</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
           <t>P1</t>
@@ -1630,7 +1670,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>P1-A11</t>
+          <t>SSF00607-P1-A11</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1665,7 +1705,11 @@
       <c r="I12" t="n">
         <v>4.34</v>
       </c>
-      <c r="J12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>P1-A11</t>
+        </is>
+      </c>
       <c r="K12" t="inlineStr">
         <is>
           <t>P1</t>
@@ -1734,7 +1778,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>P1-A12</t>
+          <t>SSF00607-P1-A12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1769,7 +1813,11 @@
       <c r="I13" t="n">
         <v>3.88</v>
       </c>
-      <c r="J13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>P1-A12</t>
+        </is>
+      </c>
       <c r="K13" t="inlineStr">
         <is>
           <t>P1</t>
@@ -1838,7 +1886,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>P1-B01</t>
+          <t>SSF00607-P1-B01</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1873,7 +1921,11 @@
       <c r="I14" t="n">
         <v>4.59</v>
       </c>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>P1-B01</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>P1</t>
@@ -1942,7 +1994,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>P1-B02</t>
+          <t>SSF00607-P1-B02</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1977,7 +2029,11 @@
       <c r="I15" t="n">
         <v>5.03</v>
       </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>P1-B02</t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr">
         <is>
           <t>P1</t>
@@ -2046,7 +2102,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>P1-B03</t>
+          <t>SSF00607-P1-B03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2081,7 +2137,11 @@
       <c r="I16" t="n">
         <v>3.06</v>
       </c>
-      <c r="J16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>P1-B03</t>
+        </is>
+      </c>
       <c r="K16" t="inlineStr">
         <is>
           <t>P1</t>
@@ -2150,7 +2210,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>P1-B04</t>
+          <t>SSF00607-P1-B04</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2185,7 +2245,11 @@
       <c r="I17" t="n">
         <v>3.13</v>
       </c>
-      <c r="J17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>P1-B04</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr">
         <is>
           <t>P1</t>
@@ -2254,7 +2318,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>P1-B05</t>
+          <t>SSF00607-P1-B05</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2289,7 +2353,11 @@
       <c r="I18" t="n">
         <v>3.06</v>
       </c>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>P1-B05</t>
+        </is>
+      </c>
       <c r="K18" t="inlineStr">
         <is>
           <t>P1</t>
@@ -2358,7 +2426,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>P1-B06</t>
+          <t>SSF00607-P1-B06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2393,7 +2461,11 @@
       <c r="I19" t="n">
         <v>3.84</v>
       </c>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>P1-B06</t>
+        </is>
+      </c>
       <c r="K19" t="inlineStr">
         <is>
           <t>P1</t>
@@ -2462,7 +2534,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>P1-B07</t>
+          <t>SSF00607-P1-B07</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2497,7 +2569,11 @@
       <c r="I20" t="n">
         <v>9.81</v>
       </c>
-      <c r="J20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>P1-B07</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr">
         <is>
           <t>P1</t>
@@ -2566,7 +2642,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>P1-B08</t>
+          <t>SSF00607-P1-B08</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2601,7 +2677,11 @@
       <c r="I21" t="n">
         <v>6.76</v>
       </c>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>P1-B08</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr">
         <is>
           <t>P1</t>
@@ -2670,7 +2750,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>P1-B09</t>
+          <t>SSF00607-P1-B09</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2705,7 +2785,11 @@
       <c r="I22" t="n">
         <v>8.279999999999999</v>
       </c>
-      <c r="J22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>P1-B09</t>
+        </is>
+      </c>
       <c r="K22" t="inlineStr">
         <is>
           <t>P1</t>
@@ -2774,7 +2858,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>P1-B10</t>
+          <t>SSF00607-P1-B10</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2809,7 +2893,11 @@
       <c r="I23" t="n">
         <v>9.26</v>
       </c>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>P1-B10</t>
+        </is>
+      </c>
       <c r="K23" t="inlineStr">
         <is>
           <t>P1</t>
@@ -2878,7 +2966,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>P1-B11</t>
+          <t>SSF00607-P1-B11</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2913,7 +3001,11 @@
       <c r="I24" t="n">
         <v>10.52</v>
       </c>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>P1-B11</t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr">
         <is>
           <t>P1</t>
@@ -2982,7 +3074,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>P1-B12</t>
+          <t>SSF00607-P1-B12</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3017,7 +3109,11 @@
       <c r="I25" t="n">
         <v>12.24</v>
       </c>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>P1-B12</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr">
         <is>
           <t>P1</t>
@@ -3086,7 +3182,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>P1-C01</t>
+          <t>SSF00607-P1-C01</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3121,7 +3217,11 @@
       <c r="I26" t="n">
         <v>8.619999999999999</v>
       </c>
-      <c r="J26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>P1-C01</t>
+        </is>
+      </c>
       <c r="K26" t="inlineStr">
         <is>
           <t>P1</t>
@@ -3190,7 +3290,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>P1-C02</t>
+          <t>SSF00607-P1-C02</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3225,7 +3325,11 @@
       <c r="I27" t="n">
         <v>8.44</v>
       </c>
-      <c r="J27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>P1-C02</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr">
         <is>
           <t>P1</t>
@@ -3294,7 +3398,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>P1-C03</t>
+          <t>SSF00607-P1-C03</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3329,7 +3433,11 @@
       <c r="I28" t="n">
         <v>8.56</v>
       </c>
-      <c r="J28" t="inlineStr"/>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>P1-C03</t>
+        </is>
+      </c>
       <c r="K28" t="inlineStr">
         <is>
           <t>P1</t>
@@ -3398,7 +3506,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>P1-C04</t>
+          <t>SSF00607-P1-C04</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3433,7 +3541,11 @@
       <c r="I29" t="n">
         <v>9.25</v>
       </c>
-      <c r="J29" t="inlineStr"/>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>P1-C04</t>
+        </is>
+      </c>
       <c r="K29" t="inlineStr">
         <is>
           <t>P1</t>
@@ -3502,7 +3614,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>P1-C05</t>
+          <t>SSF00607-P1-C05</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3537,7 +3649,11 @@
       <c r="I30" t="n">
         <v>7.97</v>
       </c>
-      <c r="J30" t="inlineStr"/>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>P1-C05</t>
+        </is>
+      </c>
       <c r="K30" t="inlineStr">
         <is>
           <t>P1</t>
@@ -3606,7 +3722,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>P1-C06</t>
+          <t>SSF00607-P1-C06</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3641,7 +3757,11 @@
       <c r="I31" t="n">
         <v>8.81</v>
       </c>
-      <c r="J31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>P1-C06</t>
+        </is>
+      </c>
       <c r="K31" t="inlineStr">
         <is>
           <t>P1</t>
@@ -3710,7 +3830,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>P1-C07</t>
+          <t>SSF00607-P1-C07</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3745,7 +3865,11 @@
       <c r="I32" t="n">
         <v>6.13</v>
       </c>
-      <c r="J32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>P1-C07</t>
+        </is>
+      </c>
       <c r="K32" t="inlineStr">
         <is>
           <t>P1</t>
@@ -3814,7 +3938,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>P1-C08</t>
+          <t>SSF00607-P1-C08</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3849,7 +3973,11 @@
       <c r="I33" t="n">
         <v>6.32</v>
       </c>
-      <c r="J33" t="inlineStr"/>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>P1-C08</t>
+        </is>
+      </c>
       <c r="K33" t="inlineStr">
         <is>
           <t>P1</t>
@@ -3918,7 +4046,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>P1-C09</t>
+          <t>SSF00607-P1-C09</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3953,7 +4081,11 @@
       <c r="I34" t="n">
         <v>6.23</v>
       </c>
-      <c r="J34" t="inlineStr"/>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>P1-C09</t>
+        </is>
+      </c>
       <c r="K34" t="inlineStr">
         <is>
           <t>P1</t>
@@ -4022,7 +4154,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>P1-C10</t>
+          <t>SSF00607-P1-C10</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4057,7 +4189,11 @@
       <c r="I35" t="n">
         <v>9.94</v>
       </c>
-      <c r="J35" t="inlineStr"/>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>P1-C10</t>
+        </is>
+      </c>
       <c r="K35" t="inlineStr">
         <is>
           <t>P1</t>
@@ -4126,7 +4262,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>P1-C11</t>
+          <t>SSF00607-P1-C11</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4161,7 +4297,11 @@
       <c r="I36" t="n">
         <v>8.68</v>
       </c>
-      <c r="J36" t="inlineStr"/>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>P1-C11</t>
+        </is>
+      </c>
       <c r="K36" t="inlineStr">
         <is>
           <t>P1</t>
@@ -4230,7 +4370,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>P1-C12</t>
+          <t>SSF00607-P1-C12</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4265,7 +4405,11 @@
       <c r="I37" t="n">
         <v>6.05</v>
       </c>
-      <c r="J37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>P1-C12</t>
+        </is>
+      </c>
       <c r="K37" t="inlineStr">
         <is>
           <t>P1</t>
@@ -4334,7 +4478,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>P1-D01</t>
+          <t>SSF00607-P1-D01</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4369,7 +4513,11 @@
       <c r="I38" t="n">
         <v>10.57</v>
       </c>
-      <c r="J38" t="inlineStr"/>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>P1-D01</t>
+        </is>
+      </c>
       <c r="K38" t="inlineStr">
         <is>
           <t>P1</t>
@@ -4438,7 +4586,7 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>P1-D02</t>
+          <t>SSF00607-P1-D02</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4473,7 +4621,11 @@
       <c r="I39" t="n">
         <v>9.880000000000001</v>
       </c>
-      <c r="J39" t="inlineStr"/>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>P1-D02</t>
+        </is>
+      </c>
       <c r="K39" t="inlineStr">
         <is>
           <t>P1</t>
@@ -4542,7 +4694,7 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>P1-D03</t>
+          <t>SSF00607-P1-D03</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4577,7 +4729,11 @@
       <c r="I40" t="n">
         <v>12.08</v>
       </c>
-      <c r="J40" t="inlineStr"/>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>P1-D03</t>
+        </is>
+      </c>
       <c r="K40" t="inlineStr">
         <is>
           <t>P1</t>
@@ -4646,7 +4802,7 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>P1-D04</t>
+          <t>SSF00607-P1-D04</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4681,7 +4837,11 @@
       <c r="I41" t="n">
         <v>10.18</v>
       </c>
-      <c r="J41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>P1-D04</t>
+        </is>
+      </c>
       <c r="K41" t="inlineStr">
         <is>
           <t>P1</t>
@@ -4750,7 +4910,7 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>P1-D05</t>
+          <t>SSF00607-P1-D05</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4785,7 +4945,11 @@
       <c r="I42" t="n">
         <v>11.52</v>
       </c>
-      <c r="J42" t="inlineStr"/>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>P1-D05</t>
+        </is>
+      </c>
       <c r="K42" t="inlineStr">
         <is>
           <t>P1</t>
@@ -4854,7 +5018,7 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>P1-D06</t>
+          <t>SSF00607-P1-D06</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4889,7 +5053,11 @@
       <c r="I43" t="n">
         <v>8.58</v>
       </c>
-      <c r="J43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>P1-D06</t>
+        </is>
+      </c>
       <c r="K43" t="inlineStr">
         <is>
           <t>P1</t>
@@ -4958,7 +5126,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>P1-D07</t>
+          <t>SSF00607-P1-D07</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -4993,7 +5161,11 @@
       <c r="I44" t="n">
         <v>4.97</v>
       </c>
-      <c r="J44" t="inlineStr"/>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>P1-D07</t>
+        </is>
+      </c>
       <c r="K44" t="inlineStr">
         <is>
           <t>P1</t>
@@ -5062,7 +5234,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>P1-D08</t>
+          <t>SSF00607-P1-D08</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5097,7 +5269,11 @@
       <c r="I45" t="n">
         <v>7.13</v>
       </c>
-      <c r="J45" t="inlineStr"/>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>P1-D08</t>
+        </is>
+      </c>
       <c r="K45" t="inlineStr">
         <is>
           <t>P1</t>
@@ -5166,7 +5342,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>P1-D09</t>
+          <t>SSF00607-P1-D09</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5201,7 +5377,11 @@
       <c r="I46" t="n">
         <v>4.26</v>
       </c>
-      <c r="J46" t="inlineStr"/>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>P1-D09</t>
+        </is>
+      </c>
       <c r="K46" t="inlineStr">
         <is>
           <t>P1</t>
@@ -5270,7 +5450,7 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>P1-D10</t>
+          <t>SSF00607-P1-D10</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5305,7 +5485,11 @@
       <c r="I47" t="n">
         <v>6.83</v>
       </c>
-      <c r="J47" t="inlineStr"/>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>P1-D10</t>
+        </is>
+      </c>
       <c r="K47" t="inlineStr">
         <is>
           <t>P1</t>
@@ -5374,7 +5558,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>P1-D11</t>
+          <t>SSF00607-P1-D11</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5409,7 +5593,11 @@
       <c r="I48" t="n">
         <v>13.61</v>
       </c>
-      <c r="J48" t="inlineStr"/>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>P1-D11</t>
+        </is>
+      </c>
       <c r="K48" t="inlineStr">
         <is>
           <t>P1</t>
@@ -5478,7 +5666,7 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>P1-D12</t>
+          <t>SSF00607-P1-D12</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5513,7 +5701,11 @@
       <c r="I49" t="n">
         <v>4.84</v>
       </c>
-      <c r="J49" t="inlineStr"/>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>P1-D12</t>
+        </is>
+      </c>
       <c r="K49" t="inlineStr">
         <is>
           <t>P1</t>
@@ -5582,7 +5774,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>P1-E01</t>
+          <t>SSF00607-P1-E01</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5617,7 +5809,11 @@
       <c r="I50" t="n">
         <v>12.99</v>
       </c>
-      <c r="J50" t="inlineStr"/>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>P1-E01</t>
+        </is>
+      </c>
       <c r="K50" t="inlineStr">
         <is>
           <t>P1</t>
@@ -5686,7 +5882,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>P1-E02</t>
+          <t>SSF00607-P1-E02</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5721,7 +5917,11 @@
       <c r="I51" t="n">
         <v>14.8</v>
       </c>
-      <c r="J51" t="inlineStr"/>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>P1-E02</t>
+        </is>
+      </c>
       <c r="K51" t="inlineStr">
         <is>
           <t>P1</t>
@@ -5790,7 +5990,7 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>P1-E03</t>
+          <t>SSF00607-P1-E03</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5825,7 +6025,11 @@
       <c r="I52" t="n">
         <v>7.89</v>
       </c>
-      <c r="J52" t="inlineStr"/>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>P1-E03</t>
+        </is>
+      </c>
       <c r="K52" t="inlineStr">
         <is>
           <t>P1</t>
@@ -5894,7 +6098,7 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>P1-E04</t>
+          <t>SSF00607-P1-E04</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5929,7 +6133,11 @@
       <c r="I53" t="n">
         <v>10.1</v>
       </c>
-      <c r="J53" t="inlineStr"/>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>P1-E04</t>
+        </is>
+      </c>
       <c r="K53" t="inlineStr">
         <is>
           <t>P1</t>
@@ -5998,7 +6206,7 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>P1-E05</t>
+          <t>SSF00607-P1-E05</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -6033,7 +6241,11 @@
       <c r="I54" t="n">
         <v>17</v>
       </c>
-      <c r="J54" t="inlineStr"/>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>P1-E05</t>
+        </is>
+      </c>
       <c r="K54" t="inlineStr">
         <is>
           <t>P1</t>
@@ -6102,7 +6314,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>P1-E06</t>
+          <t>SSF00607-P1-E06</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -6137,7 +6349,11 @@
       <c r="I55" t="n">
         <v>12.57</v>
       </c>
-      <c r="J55" t="inlineStr"/>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>P1-E06</t>
+        </is>
+      </c>
       <c r="K55" t="inlineStr">
         <is>
           <t>P1</t>
@@ -6206,7 +6422,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>P1-E07</t>
+          <t>SSF00607-P1-E07</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -6241,7 +6457,11 @@
       <c r="I56" t="n">
         <v>7.67</v>
       </c>
-      <c r="J56" t="inlineStr"/>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>P1-E07</t>
+        </is>
+      </c>
       <c r="K56" t="inlineStr">
         <is>
           <t>P1</t>
@@ -6310,7 +6530,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>P1-E08</t>
+          <t>SSF00607-P1-E08</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -6345,7 +6565,11 @@
       <c r="I57" t="n">
         <v>9.1</v>
       </c>
-      <c r="J57" t="inlineStr"/>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>P1-E08</t>
+        </is>
+      </c>
       <c r="K57" t="inlineStr">
         <is>
           <t>P1</t>
@@ -6414,7 +6638,7 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>P1-E09</t>
+          <t>SSF00607-P1-E09</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -6449,7 +6673,11 @@
       <c r="I58" t="n">
         <v>7.04</v>
       </c>
-      <c r="J58" t="inlineStr"/>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>P1-E09</t>
+        </is>
+      </c>
       <c r="K58" t="inlineStr">
         <is>
           <t>P1</t>
@@ -6518,7 +6746,7 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>P1-E10</t>
+          <t>SSF00607-P1-E10</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -6553,7 +6781,11 @@
       <c r="I59" t="n">
         <v>9.06</v>
       </c>
-      <c r="J59" t="inlineStr"/>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>P1-E10</t>
+        </is>
+      </c>
       <c r="K59" t="inlineStr">
         <is>
           <t>P1</t>
@@ -6622,7 +6854,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>P1-E11</t>
+          <t>SSF00607-P1-E11</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -6657,7 +6889,11 @@
       <c r="I60" t="n">
         <v>8.66</v>
       </c>
-      <c r="J60" t="inlineStr"/>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>P1-E11</t>
+        </is>
+      </c>
       <c r="K60" t="inlineStr">
         <is>
           <t>P1</t>
@@ -6726,7 +6962,7 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>P1-E12</t>
+          <t>SSF00607-P1-E12</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -6761,7 +6997,11 @@
       <c r="I61" t="n">
         <v>7.24</v>
       </c>
-      <c r="J61" t="inlineStr"/>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>P1-E12</t>
+        </is>
+      </c>
       <c r="K61" t="inlineStr">
         <is>
           <t>P1</t>
@@ -6830,7 +7070,7 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>P1-F01</t>
+          <t>SSF00607-P1-F01</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -6865,7 +7105,11 @@
       <c r="I62" t="n">
         <v>10.43</v>
       </c>
-      <c r="J62" t="inlineStr"/>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>P1-F01</t>
+        </is>
+      </c>
       <c r="K62" t="inlineStr">
         <is>
           <t>P1</t>
@@ -6934,7 +7178,7 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>P1-F02</t>
+          <t>SSF00607-P1-F02</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -6969,7 +7213,11 @@
       <c r="I63" t="n">
         <v>9.9</v>
       </c>
-      <c r="J63" t="inlineStr"/>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>P1-F02</t>
+        </is>
+      </c>
       <c r="K63" t="inlineStr">
         <is>
           <t>P1</t>
@@ -7038,7 +7286,7 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>P1-F03</t>
+          <t>SSF00607-P1-F03</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -7073,7 +7321,11 @@
       <c r="I64" t="n">
         <v>10.32</v>
       </c>
-      <c r="J64" t="inlineStr"/>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>P1-F03</t>
+        </is>
+      </c>
       <c r="K64" t="inlineStr">
         <is>
           <t>P1</t>
@@ -7142,7 +7394,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>P1-F04</t>
+          <t>SSF00607-P1-F04</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -7177,7 +7429,11 @@
       <c r="I65" t="n">
         <v>7.33</v>
       </c>
-      <c r="J65" t="inlineStr"/>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>P1-F04</t>
+        </is>
+      </c>
       <c r="K65" t="inlineStr">
         <is>
           <t>P1</t>
@@ -7246,7 +7502,7 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>P1-F05</t>
+          <t>SSF00607-P1-F05</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -7281,7 +7537,11 @@
       <c r="I66" t="n">
         <v>14.73</v>
       </c>
-      <c r="J66" t="inlineStr"/>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>P1-F05</t>
+        </is>
+      </c>
       <c r="K66" t="inlineStr">
         <is>
           <t>P1</t>
@@ -7350,7 +7610,7 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>P1-F06</t>
+          <t>SSF00607-P1-F06</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -7385,7 +7645,11 @@
       <c r="I67" t="n">
         <v>9.93</v>
       </c>
-      <c r="J67" t="inlineStr"/>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>P1-F06</t>
+        </is>
+      </c>
       <c r="K67" t="inlineStr">
         <is>
           <t>P1</t>
@@ -7454,7 +7718,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>P1-F07</t>
+          <t>SSF00607-P1-F07</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -7489,7 +7753,11 @@
       <c r="I68" t="n">
         <v>11.1</v>
       </c>
-      <c r="J68" t="inlineStr"/>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>P1-F07</t>
+        </is>
+      </c>
       <c r="K68" t="inlineStr">
         <is>
           <t>P1</t>
@@ -7558,7 +7826,7 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>P1-F08</t>
+          <t>SSF00607-P1-F08</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -7593,7 +7861,11 @@
       <c r="I69" t="n">
         <v>5.61</v>
       </c>
-      <c r="J69" t="inlineStr"/>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>P1-F08</t>
+        </is>
+      </c>
       <c r="K69" t="inlineStr">
         <is>
           <t>P1</t>
@@ -7662,7 +7934,7 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>P1-F09</t>
+          <t>SSF00607-P1-F09</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -7697,7 +7969,11 @@
       <c r="I70" t="n">
         <v>8.31</v>
       </c>
-      <c r="J70" t="inlineStr"/>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>P1-F09</t>
+        </is>
+      </c>
       <c r="K70" t="inlineStr">
         <is>
           <t>P1</t>
@@ -7766,7 +8042,7 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>P1-F10</t>
+          <t>SSF00607-P1-F10</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -7801,7 +8077,11 @@
       <c r="I71" t="n">
         <v>8.65</v>
       </c>
-      <c r="J71" t="inlineStr"/>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>P1-F10</t>
+        </is>
+      </c>
       <c r="K71" t="inlineStr">
         <is>
           <t>P1</t>
@@ -7870,7 +8150,7 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>P1-F11</t>
+          <t>SSF00607-P1-F11</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -7905,7 +8185,11 @@
       <c r="I72" t="n">
         <v>9.210000000000001</v>
       </c>
-      <c r="J72" t="inlineStr"/>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>P1-F11</t>
+        </is>
+      </c>
       <c r="K72" t="inlineStr">
         <is>
           <t>P1</t>
@@ -7974,7 +8258,7 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>P1-F12</t>
+          <t>SSF00607-P1-F12</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -8009,7 +8293,11 @@
       <c r="I73" t="n">
         <v>11.16</v>
       </c>
-      <c r="J73" t="inlineStr"/>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>P1-F12</t>
+        </is>
+      </c>
       <c r="K73" t="inlineStr">
         <is>
           <t>P1</t>
@@ -8078,7 +8366,7 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>P1-G01</t>
+          <t>SSF00607-P1-G01</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -8113,7 +8401,11 @@
       <c r="I74" t="n">
         <v>13.38</v>
       </c>
-      <c r="J74" t="inlineStr"/>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>P1-G01</t>
+        </is>
+      </c>
       <c r="K74" t="inlineStr">
         <is>
           <t>P1</t>
@@ -8182,7 +8474,7 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>P1-G02</t>
+          <t>SSF00607-P1-G02</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -8217,7 +8509,11 @@
       <c r="I75" t="n">
         <v>10.81</v>
       </c>
-      <c r="J75" t="inlineStr"/>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>P1-G02</t>
+        </is>
+      </c>
       <c r="K75" t="inlineStr">
         <is>
           <t>P1</t>
@@ -8286,7 +8582,7 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>P1-G03</t>
+          <t>SSF00607-P1-G03</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -8321,7 +8617,11 @@
       <c r="I76" t="n">
         <v>13.76</v>
       </c>
-      <c r="J76" t="inlineStr"/>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>P1-G03</t>
+        </is>
+      </c>
       <c r="K76" t="inlineStr">
         <is>
           <t>P1</t>
@@ -8390,7 +8690,7 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>P1-G04</t>
+          <t>SSF00607-P1-G04</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -8425,7 +8725,11 @@
       <c r="I77" t="n">
         <v>12.3</v>
       </c>
-      <c r="J77" t="inlineStr"/>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>P1-G04</t>
+        </is>
+      </c>
       <c r="K77" t="inlineStr">
         <is>
           <t>P1</t>
@@ -8494,7 +8798,7 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>P1-G05</t>
+          <t>SSF00607-P1-G05</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -8529,7 +8833,11 @@
       <c r="I78" t="n">
         <v>13.98</v>
       </c>
-      <c r="J78" t="inlineStr"/>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>P1-G05</t>
+        </is>
+      </c>
       <c r="K78" t="inlineStr">
         <is>
           <t>P1</t>
@@ -8598,7 +8906,7 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>P1-G06</t>
+          <t>SSF00607-P1-G06</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -8633,7 +8941,11 @@
       <c r="I79" t="n">
         <v>13.57</v>
       </c>
-      <c r="J79" t="inlineStr"/>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>P1-G06</t>
+        </is>
+      </c>
       <c r="K79" t="inlineStr">
         <is>
           <t>P1</t>
@@ -8702,7 +9014,7 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>P1-G07</t>
+          <t>SSF00607-P1-G07</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -8737,7 +9049,11 @@
       <c r="I80" t="n">
         <v>13.76</v>
       </c>
-      <c r="J80" t="inlineStr"/>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>P1-G07</t>
+        </is>
+      </c>
       <c r="K80" t="inlineStr">
         <is>
           <t>P1</t>
@@ -8806,7 +9122,7 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>P1-G08</t>
+          <t>SSF00607-P1-G08</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -8841,7 +9157,11 @@
       <c r="I81" t="n">
         <v>14.95</v>
       </c>
-      <c r="J81" t="inlineStr"/>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>P1-G08</t>
+        </is>
+      </c>
       <c r="K81" t="inlineStr">
         <is>
           <t>P1</t>
@@ -8910,7 +9230,7 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>P1-G09</t>
+          <t>SSF00607-P1-G09</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -8945,7 +9265,11 @@
       <c r="I82" t="n">
         <v>15.08</v>
       </c>
-      <c r="J82" t="inlineStr"/>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>P1-G09</t>
+        </is>
+      </c>
       <c r="K82" t="inlineStr">
         <is>
           <t>P1</t>
@@ -9014,7 +9338,7 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>P1-G10</t>
+          <t>SSF00607-P1-G10</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -9049,7 +9373,11 @@
       <c r="I83" t="n">
         <v>15.28</v>
       </c>
-      <c r="J83" t="inlineStr"/>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>P1-G10</t>
+        </is>
+      </c>
       <c r="K83" t="inlineStr">
         <is>
           <t>P1</t>
@@ -9118,7 +9446,7 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>P1-G11</t>
+          <t>SSF00607-P1-G11</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -9153,7 +9481,11 @@
       <c r="I84" t="n">
         <v>15.67</v>
       </c>
-      <c r="J84" t="inlineStr"/>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>P1-G11</t>
+        </is>
+      </c>
       <c r="K84" t="inlineStr">
         <is>
           <t>P1</t>
@@ -9222,7 +9554,7 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>P1-G12</t>
+          <t>SSF00607-P1-G12</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -9257,7 +9589,11 @@
       <c r="I85" t="n">
         <v>16.34</v>
       </c>
-      <c r="J85" t="inlineStr"/>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>P1-G12</t>
+        </is>
+      </c>
       <c r="K85" t="inlineStr">
         <is>
           <t>P1</t>
@@ -9326,7 +9662,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>P1-H01</t>
+          <t>SSF00607-P1-H01</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -9355,7 +9691,11 @@
         <v>250</v>
       </c>
       <c r="I86" t="inlineStr"/>
-      <c r="J86" t="inlineStr"/>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>P1-H01</t>
+        </is>
+      </c>
       <c r="K86" t="inlineStr">
         <is>
           <t>P1</t>
@@ -9422,7 +9762,7 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>P1-H02</t>
+          <t>SSF00607-P1-H02</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -9451,7 +9791,11 @@
         <v>250</v>
       </c>
       <c r="I87" t="inlineStr"/>
-      <c r="J87" t="inlineStr"/>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>P1-H02</t>
+        </is>
+      </c>
       <c r="K87" t="inlineStr">
         <is>
           <t>P1</t>
@@ -9518,7 +9862,7 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>P1-H03</t>
+          <t>SSF00607-P1-H03</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -9547,7 +9891,11 @@
         <v>250</v>
       </c>
       <c r="I88" t="inlineStr"/>
-      <c r="J88" t="inlineStr"/>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>P1-H03</t>
+        </is>
+      </c>
       <c r="K88" t="inlineStr">
         <is>
           <t>P1</t>
@@ -9614,7 +9962,7 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>P1-H04</t>
+          <t>SSF00607-P1-H04</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -9643,7 +9991,11 @@
         <v>250</v>
       </c>
       <c r="I89" t="inlineStr"/>
-      <c r="J89" t="inlineStr"/>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>P1-H04</t>
+        </is>
+      </c>
       <c r="K89" t="inlineStr">
         <is>
           <t>P1</t>
@@ -9710,7 +10062,7 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>P1-H05</t>
+          <t>SSF00607-P1-H05</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -9739,7 +10091,11 @@
         <v>250</v>
       </c>
       <c r="I90" t="inlineStr"/>
-      <c r="J90" t="inlineStr"/>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>P1-H05</t>
+        </is>
+      </c>
       <c r="K90" t="inlineStr">
         <is>
           <t>P1</t>
@@ -9806,7 +10162,7 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>P1-H06</t>
+          <t>SSF00607-P1-H06</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -9835,7 +10191,11 @@
         <v>250</v>
       </c>
       <c r="I91" t="inlineStr"/>
-      <c r="J91" t="inlineStr"/>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>P1-H06</t>
+        </is>
+      </c>
       <c r="K91" t="inlineStr">
         <is>
           <t>P1</t>
@@ -9902,7 +10262,7 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>P1-H07</t>
+          <t>SSF00607-P1-H07</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -9931,7 +10291,11 @@
         <v>250</v>
       </c>
       <c r="I92" t="inlineStr"/>
-      <c r="J92" t="inlineStr"/>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>P1-H07</t>
+        </is>
+      </c>
       <c r="K92" t="inlineStr">
         <is>
           <t>P1</t>
@@ -9998,7 +10362,7 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>P1-H08</t>
+          <t>SSF00607-P1-H08</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -10027,7 +10391,11 @@
         <v>250</v>
       </c>
       <c r="I93" t="inlineStr"/>
-      <c r="J93" t="inlineStr"/>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>P1-H08</t>
+        </is>
+      </c>
       <c r="K93" t="inlineStr">
         <is>
           <t>P1</t>
@@ -10094,7 +10462,7 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>P1-H09</t>
+          <t>SSF00607-P1-H09</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -10123,7 +10491,11 @@
         <v>250</v>
       </c>
       <c r="I94" t="inlineStr"/>
-      <c r="J94" t="inlineStr"/>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>P1-H09</t>
+        </is>
+      </c>
       <c r="K94" t="inlineStr">
         <is>
           <t>P1</t>
@@ -10190,7 +10562,7 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>P1-H10</t>
+          <t>SSF00607-P1-H10</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -10219,7 +10591,11 @@
         <v>250</v>
       </c>
       <c r="I95" t="inlineStr"/>
-      <c r="J95" t="inlineStr"/>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>P1-H10</t>
+        </is>
+      </c>
       <c r="K95" t="inlineStr">
         <is>
           <t>P1</t>
@@ -10286,7 +10662,7 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>P1-H11</t>
+          <t>SSF00607-P1-H11</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -10315,7 +10691,11 @@
         <v>250</v>
       </c>
       <c r="I96" t="inlineStr"/>
-      <c r="J96" t="inlineStr"/>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>P1-H11</t>
+        </is>
+      </c>
       <c r="K96" t="inlineStr">
         <is>
           <t>P1</t>
@@ -10382,7 +10762,7 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>P1-H12</t>
+          <t>SSF00607-P1-H12</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -10411,7 +10791,11 @@
         <v>250</v>
       </c>
       <c r="I97" t="inlineStr"/>
-      <c r="J97" t="inlineStr"/>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>P1-H12</t>
+        </is>
+      </c>
       <c r="K97" t="inlineStr">
         <is>
           <t>P1</t>

</xml_diff>